<commit_message>
Modified Sign Extender and Added more comments
</commit_message>
<xml_diff>
--- a/CPU_NN/ouput matching/CPUOUtputEqualTest.xlsx
+++ b/CPU_NN/ouput matching/CPUOUtputEqualTest.xlsx
@@ -11,22 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <definedNames>
+    <definedName name="List1">Sheet1!$A:$A</definedName>
+    <definedName name="List2">Sheet1!$B:$B</definedName>
+  </definedNames>
   <calcPr calcId="145621"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>CPU output</t>
-  </si>
-  <si>
-    <t>Computed Result</t>
-  </si>
-  <si>
-    <t>Equal??</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -379,10 +369,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4001"/>
+  <dimension ref="A1:D4001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+      <selection activeCell="B2" sqref="B2:B4001"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -391,18 +381,12 @@
     <col min="2" max="2" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1"/>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -413,8 +397,12 @@
         <f>A2=B2</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2" t="b">
+        <f>List1=List2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -426,7 +414,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -438,7 +426,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1</v>
       </c>
@@ -450,7 +438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -462,7 +450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -474,7 +462,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -486,7 +474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -498,7 +486,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -510,7 +498,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1</v>
       </c>
@@ -522,7 +510,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1</v>
       </c>
@@ -534,7 +522,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
@@ -546,7 +534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>0</v>
       </c>
@@ -558,7 +546,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1</v>
       </c>
@@ -570,7 +558,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>1</v>
       </c>

</xml_diff>